<commit_message>
uploade dthe filesform the 3 to the 18 of November
</commit_message>
<xml_diff>
--- a/files/Matières/EPS/T1/001 Course de demi-fond Bac Général et technologique 2020.xlsx
+++ b/files/Matières/EPS/T1/001 Course de demi-fond Bac Général et technologique 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry PC\Documents\001 Github prog Sharing\Backup-of-matiere\files\Matières\EPS\T1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D513AF6E-5B39-4B82-8CF6-D1E7A4372BCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2E86A9F-7F01-46A9-9811-4C5186F63753}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -603,6 +604,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -621,12 +631,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -636,13 +640,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -925,795 +926,798 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B2:W27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
       <selection activeCell="R12" sqref="R12:S16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.06640625" style="1"/>
+    <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:23" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="3" spans="2:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="13" t="s">
+    <row r="2" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="2" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="4"/>
-    </row>
-    <row r="4" spans="2:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="2" t="s">
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="7"/>
+    </row>
+    <row r="4" spans="2:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="7"/>
-    </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.45">
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="7"/>
-    </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.45">
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="7"/>
-    </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.45">
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="7"/>
-    </row>
-    <row r="8" spans="2:23" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="5" t="s">
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="10"/>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="10"/>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="10"/>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="10"/>
+    </row>
+    <row r="8" spans="2:23" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="5" t="s">
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6" t="s">
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
-      <c r="W8" s="7"/>
-    </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.45">
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="7"/>
-    </row>
-    <row r="10" spans="2:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="5" t="s">
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="10"/>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="10"/>
+    </row>
+    <row r="10" spans="2:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="5" t="s">
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6" t="s">
+      <c r="G10" s="9"/>
+      <c r="H10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6" t="s">
+      <c r="I10" s="9"/>
+      <c r="J10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6" t="s">
+      <c r="K10" s="9"/>
+      <c r="L10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6" t="s">
+      <c r="M10" s="9"/>
+      <c r="N10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6" t="s">
+      <c r="O10" s="9"/>
+      <c r="P10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6" t="s">
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6" t="s">
+      <c r="S10" s="9"/>
+      <c r="T10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6" t="s">
+      <c r="U10" s="9"/>
+      <c r="V10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="W10" s="7"/>
-    </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.45">
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="7"/>
-    </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.45">
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="5">
+      <c r="W10" s="10"/>
+    </row>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="10"/>
+    </row>
+    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="8">
         <v>0.7</v>
       </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6" t="s">
+      <c r="G12" s="9"/>
+      <c r="H12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6" t="s">
+      <c r="I12" s="9"/>
+      <c r="J12" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6">
+      <c r="K12" s="9"/>
+      <c r="L12" s="9">
         <v>7</v>
       </c>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6" t="s">
+      <c r="M12" s="9"/>
+      <c r="N12" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6" t="s">
+      <c r="O12" s="9"/>
+      <c r="P12" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6">
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9">
         <v>11.2</v>
       </c>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6" t="s">
+      <c r="S12" s="9"/>
+      <c r="T12" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6" t="s">
+      <c r="U12" s="9"/>
+      <c r="V12" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="W12" s="7"/>
-    </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.45">
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="5">
+      <c r="W12" s="10"/>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="8">
         <v>1.4</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6" t="s">
+      <c r="G13" s="9"/>
+      <c r="H13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6" t="s">
+      <c r="I13" s="9"/>
+      <c r="J13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6">
+      <c r="K13" s="9"/>
+      <c r="L13" s="9">
         <v>7.7</v>
       </c>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6" t="s">
+      <c r="M13" s="9"/>
+      <c r="N13" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6" t="s">
+      <c r="O13" s="9"/>
+      <c r="P13" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6">
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9">
         <v>11.9</v>
       </c>
-      <c r="S13" s="6"/>
-      <c r="T13" s="6" t="s">
+      <c r="S13" s="9"/>
+      <c r="T13" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="U13" s="6"/>
-      <c r="V13" s="6" t="s">
+      <c r="U13" s="9"/>
+      <c r="V13" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="W13" s="7"/>
-    </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.45">
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="5">
+      <c r="W13" s="10"/>
+    </row>
+    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="8">
         <v>2.1</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6" t="s">
+      <c r="G14" s="9"/>
+      <c r="H14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6" t="s">
+      <c r="I14" s="9"/>
+      <c r="J14" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6">
+      <c r="K14" s="9"/>
+      <c r="L14" s="9">
         <v>8.4</v>
       </c>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6" t="s">
+      <c r="M14" s="9"/>
+      <c r="N14" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6" t="s">
+      <c r="O14" s="9"/>
+      <c r="P14" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6">
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9">
         <v>12.6</v>
       </c>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6" t="s">
+      <c r="S14" s="9"/>
+      <c r="T14" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="U14" s="6"/>
-      <c r="V14" s="6" t="s">
+      <c r="U14" s="9"/>
+      <c r="V14" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="W14" s="7"/>
-    </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.45">
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="5">
+      <c r="W14" s="10"/>
+    </row>
+    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="8">
         <v>2.8</v>
       </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6" t="s">
+      <c r="G15" s="9"/>
+      <c r="H15" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6" t="s">
+      <c r="I15" s="9"/>
+      <c r="J15" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6">
+      <c r="K15" s="9"/>
+      <c r="L15" s="9">
         <v>9.1</v>
       </c>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6" t="s">
+      <c r="M15" s="9"/>
+      <c r="N15" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6" t="s">
+      <c r="O15" s="9"/>
+      <c r="P15" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6">
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9">
         <v>13.3</v>
       </c>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6" t="s">
+      <c r="S15" s="9"/>
+      <c r="T15" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="U15" s="6"/>
-      <c r="V15" s="6" t="s">
+      <c r="U15" s="9"/>
+      <c r="V15" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="W15" s="7"/>
-    </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.45">
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="5">
+      <c r="W15" s="10"/>
+    </row>
+    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="8">
         <v>3.5</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6" t="s">
+      <c r="G16" s="9"/>
+      <c r="H16" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6" t="s">
+      <c r="I16" s="9"/>
+      <c r="J16" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6">
+      <c r="K16" s="9"/>
+      <c r="L16" s="9">
         <v>9.8000000000000007</v>
       </c>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6" t="s">
+      <c r="M16" s="9"/>
+      <c r="N16" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6" t="s">
+      <c r="O16" s="9"/>
+      <c r="P16" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6">
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9">
         <v>14</v>
       </c>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6">
+      <c r="S16" s="9"/>
+      <c r="T16" s="9">
         <v>5.25</v>
       </c>
-      <c r="U16" s="6"/>
-      <c r="V16" s="6" t="s">
+      <c r="U16" s="9"/>
+      <c r="V16" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="W16" s="7"/>
-    </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.45">
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="5">
+      <c r="W16" s="10"/>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="8">
         <v>4.2</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6" t="s">
+      <c r="G17" s="9"/>
+      <c r="H17" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6" t="s">
+      <c r="I17" s="9"/>
+      <c r="J17" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6">
+      <c r="K17" s="9"/>
+      <c r="L17" s="9">
         <v>10.5</v>
       </c>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6" t="s">
+      <c r="M17" s="9"/>
+      <c r="N17" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6" t="s">
+      <c r="O17" s="9"/>
+      <c r="P17" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="9"/>
-    </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.45">
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="5">
+      <c r="Q17" s="9"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="14"/>
+      <c r="U17" s="14"/>
+      <c r="V17" s="14"/>
+      <c r="W17" s="15"/>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="8">
         <v>4.9000000000000004</v>
       </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6" t="s">
+      <c r="G18" s="9"/>
+      <c r="H18" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6" t="s">
+      <c r="I18" s="9"/>
+      <c r="J18" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="K18" s="6"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="8"/>
-      <c r="V18" s="8"/>
-      <c r="W18" s="9"/>
-    </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.45">
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="5">
+      <c r="K18" s="9"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="14"/>
+      <c r="W18" s="15"/>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="8">
         <v>5.6</v>
       </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6" t="s">
+      <c r="G19" s="9"/>
+      <c r="H19" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6" t="s">
+      <c r="I19" s="9"/>
+      <c r="J19" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="K19" s="6"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
-      <c r="T19" s="8"/>
-      <c r="U19" s="8"/>
-      <c r="V19" s="8"/>
-      <c r="W19" s="9"/>
-    </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.45">
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="5">
+      <c r="K19" s="9"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="14"/>
+      <c r="U19" s="14"/>
+      <c r="V19" s="14"/>
+      <c r="W19" s="15"/>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="8">
         <v>6.3</v>
       </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6" t="s">
+      <c r="G20" s="9"/>
+      <c r="H20" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6" t="s">
+      <c r="I20" s="9"/>
+      <c r="J20" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="K20" s="6"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
-      <c r="T20" s="8"/>
-      <c r="U20" s="8"/>
-      <c r="V20" s="8"/>
-      <c r="W20" s="9"/>
-    </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.45">
-      <c r="B21" s="5" t="s">
+      <c r="K20" s="9"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
+      <c r="U20" s="14"/>
+      <c r="V20" s="14"/>
+      <c r="W20" s="15"/>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="5" t="s">
+      <c r="D21" s="9"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6" t="s">
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6" t="s">
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="6"/>
-      <c r="V21" s="6"/>
-      <c r="W21" s="7"/>
-    </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.45">
-      <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
-      <c r="S22" s="6"/>
-      <c r="T22" s="6"/>
-      <c r="U22" s="6"/>
-      <c r="V22" s="6"/>
-      <c r="W22" s="7"/>
-    </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.45">
-      <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="6"/>
-      <c r="S23" s="6"/>
-      <c r="T23" s="6"/>
-      <c r="U23" s="6"/>
-      <c r="V23" s="6"/>
-      <c r="W23" s="7"/>
-    </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.45">
-      <c r="B24" s="5" t="s">
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="10"/>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B22" s="8"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="10"/>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B23" s="8"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="10"/>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="5" t="s">
+      <c r="D24" s="9"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6" t="s">
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="6" t="s">
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="S24" s="6"/>
-      <c r="T24" s="6"/>
-      <c r="U24" s="6"/>
-      <c r="V24" s="6"/>
-      <c r="W24" s="7"/>
-    </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.45">
-      <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
-      <c r="S25" s="6"/>
-      <c r="T25" s="6"/>
-      <c r="U25" s="6"/>
-      <c r="V25" s="6"/>
-      <c r="W25" s="7"/>
-    </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.45">
-      <c r="B26" s="5"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="6"/>
-      <c r="R26" s="6"/>
-      <c r="S26" s="6"/>
-      <c r="T26" s="6"/>
-      <c r="U26" s="6"/>
-      <c r="V26" s="6"/>
-      <c r="W26" s="7"/>
-    </row>
-    <row r="27" spans="2:23" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B27" s="10"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="11"/>
-      <c r="S27" s="11"/>
-      <c r="T27" s="11"/>
-      <c r="U27" s="11"/>
-      <c r="V27" s="11"/>
-      <c r="W27" s="12"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="10"/>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B25" s="8"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="10"/>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B26" s="8"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
+      <c r="W26" s="10"/>
+    </row>
+    <row r="27" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="11"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="12"/>
+      <c r="U27" s="12"/>
+      <c r="V27" s="12"/>
+      <c r="W27" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="110">
@@ -1764,38 +1768,18 @@
     <mergeCell ref="N17:O17"/>
     <mergeCell ref="N18:O18"/>
     <mergeCell ref="N19:O19"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="L15:M15"/>
     <mergeCell ref="L16:M16"/>
     <mergeCell ref="L17:M17"/>
     <mergeCell ref="L18:M18"/>
     <mergeCell ref="L19:M19"/>
     <mergeCell ref="L20:M20"/>
     <mergeCell ref="J20:K20"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="J16:K16"/>
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="J18:K18"/>
     <mergeCell ref="J19:K19"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="H13:I13"/>
     <mergeCell ref="L8:W9"/>
     <mergeCell ref="F8:K9"/>
     <mergeCell ref="F12:G12"/>
@@ -1813,23 +1797,43 @@
     <mergeCell ref="L10:M11"/>
     <mergeCell ref="J10:K11"/>
     <mergeCell ref="H10:I11"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C21:E23"/>
+    <mergeCell ref="C24:E27"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:E9"/>
+    <mergeCell ref="B21:B23"/>
     <mergeCell ref="B10:B20"/>
     <mergeCell ref="C10:E20"/>
     <mergeCell ref="F10:G11"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C21:E23"/>
-    <mergeCell ref="C24:E27"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:E9"/>
-    <mergeCell ref="B21:B23"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="70" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>